<commit_message>
Chore. sheetName 지정 가능하게 ParseOptions 타입 수정, 로직 수정
</commit_message>
<xml_diff>
--- a/test/test_data.xlsx
+++ b/test/test_data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sehoon/work/npm-modules/excel-reflect-parser/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sehoon/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C1D51B-74C4-074A-BDE7-9360AFE19BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6AC7C2-E4A8-7347-AE64-02EB71E6332D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4460" yWindow="1100" windowWidth="28100" windowHeight="16380" xr2:uid="{7465476C-5740-C84D-A405-A7F09C0EE30D}"/>
+    <workbookView xWindow="700" yWindow="500" windowWidth="28100" windowHeight="16380" xr2:uid="{7465476C-5740-C84D-A405-A7F09C0EE30D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="시트러스" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>상품ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,6 +63,26 @@
   </si>
   <si>
     <t>B23345123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마바사아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자차카타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파하</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B12345124</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B23345125</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -432,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F10CDC-0BC8-AC4F-9891-DAA1F8BE07D3}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -475,6 +496,93 @@
       <c r="A3" s="1">
         <v>1002</v>
       </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>1003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>1004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>12000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C02B3748-BB04-1345-90C2-89266FC495C3}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1002</v>
+      </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>

</xml_diff>